<commit_message>
next: continue with generate_practice_times_2, don't need sepatate method, just add the memb scheds to practice one by one (in the inner arrays)
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seasy/Documents/Projects/PM-Replacement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACA45E6-F243-5841-B938-3A644A9B6FD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22424BB2-284D-B944-B3CF-C18734B1DD0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{D0A65B29-C4AD-3F43-ADB3-EAE2E589548A}"/>
+    <workbookView xWindow="45760" yWindow="-4380" windowWidth="34900" windowHeight="22460" xr2:uid="{D0A65B29-C4AD-3F43-ADB3-EAE2E589548A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet5" sheetId="7" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="160">
   <si>
     <t>TWICE (9) - FEEL SPECIAL [SEMI-RUSH] - DUE THURS SEP 26 9:00PM</t>
   </si>
@@ -489,9 +489,6 @@
     <t>After 4h</t>
   </si>
   <si>
-    <t>Not Available (for Feb 5) Sinon free after 4h30</t>
-  </si>
-  <si>
     <t>After 5h</t>
   </si>
   <si>
@@ -504,22 +501,25 @@
     <t>I usually work on Saturdays in Brossard so it's harder for me to make it to practice if they are dt ;-; I will also be working on the 9th and 16th (2 Sundays) at Brossard too but I can try to make it if ever practice is schedule then (usually end around 6 at work so should be dt around 7:30)</t>
   </si>
   <si>
-    <t>michelle f</t>
-  </si>
-  <si>
-    <t>after 6</t>
-  </si>
-  <si>
-    <t>im in Los Angeles from feb 16-25!!!:( BUT IF WE CAN DO IT BEFORE I LEAVE PLS PICK ME KDNXNDKZ</t>
-  </si>
-  <si>
     <t>[RUSHED] BTS - BLACK SWAN (7) - DUE FRI JAN 31 9:00AM</t>
   </si>
   <si>
-    <t>Free except 4h45-6h15</t>
-  </si>
-  <si>
     <t>I also have stroke MAIS YA PLZ PICK ME IM UWU (also nics dont kill ur knees 👀👀👀👀👀) BUTTT IM FREE ALL DAY feb. 8</t>
+  </si>
+  <si>
+    <t>Quynh-Nhi</t>
+  </si>
+  <si>
+    <t>Karen</t>
+  </si>
+  <si>
+    <t>After 3:30</t>
+  </si>
+  <si>
+    <t>Free except 4h30-6h30</t>
+  </si>
+  <si>
+    <t>free after 4h30</t>
   </si>
 </sst>
 </file>
@@ -923,10 +923,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEDDD130-3FEA-B342-AB58-23B2E7542398}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -942,7 +942,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1075,27 +1075,27 @@
         <v>148</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>104</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>158</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>68</v>
@@ -1116,36 +1116,59 @@
         <v>47</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>156</v>
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
next todo: get_practice_range printing who's missing
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seasy/Documents/Projects/PM-Replacement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22424BB2-284D-B944-B3CF-C18734B1DD0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5173D31A-5894-6342-BA33-8625954E0FB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45760" yWindow="-4380" windowWidth="34900" windowHeight="22460" xr2:uid="{D0A65B29-C4AD-3F43-ADB3-EAE2E589548A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{D0A65B29-C4AD-3F43-ADB3-EAE2E589548A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet5" sheetId="7" r:id="rId1"/>
-    <sheet name="Sheet4 (2)" sheetId="6" r:id="rId2"/>
-    <sheet name="Sheet4" sheetId="5" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet name="4" sheetId="4" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId7"/>
+    <sheet name="Sheet6" sheetId="8" r:id="rId1"/>
+    <sheet name="Sheet5" sheetId="7" r:id="rId2"/>
+    <sheet name="Sheet4 (2)" sheetId="6" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId5"/>
+    <sheet name="4" sheetId="4" r:id="rId6"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId7"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="178">
   <si>
     <t>TWICE (9) - FEEL SPECIAL [SEMI-RUSH] - DUE THURS SEP 26 9:00PM</t>
   </si>
@@ -450,76 +451,153 @@
     <t>free except 3-6</t>
   </si>
   <si>
-    <t>Nic</t>
-  </si>
-  <si>
-    <t>After 5:30 PM</t>
-  </si>
-  <si>
-    <t>After 7:00 PM (most likely)</t>
-  </si>
-  <si>
-    <t>After 7:30 PM</t>
-  </si>
-  <si>
-    <t>After 6:00 PM (Not Available on Feb 7)</t>
-  </si>
-  <si>
-    <t>So like, I'm so ready to teach this! KEEPING THE BTS STREAK! CHOOSE ME!</t>
-  </si>
-  <si>
-    <t>Elany</t>
-  </si>
-  <si>
-    <t>After 7:30PM</t>
-  </si>
-  <si>
-    <t>After 1PM</t>
-  </si>
-  <si>
-    <t>*** Thursday schedule varies. Feb 6 (before 12PM), Feb 13 (1-4:30PM). *** Also, STROKE practices.</t>
-  </si>
-  <si>
-    <t>I have weki meki (February 5th and 7th) and we will be done in February 9th. I don't have school this session soooooo IM FREEEEEE HEHEHHEHE</t>
-  </si>
-  <si>
-    <t>FREE AS A BIRD</t>
-  </si>
-  <si>
-    <t>After 4h</t>
-  </si>
-  <si>
-    <t>After 5h</t>
-  </si>
-  <si>
-    <t>Shu :")</t>
-  </si>
-  <si>
-    <t>After 8</t>
-  </si>
-  <si>
-    <t>I usually work on Saturdays in Brossard so it's harder for me to make it to practice if they are dt ;-; I will also be working on the 9th and 16th (2 Sundays) at Brossard too but I can try to make it if ever practice is schedule then (usually end around 6 at work so should be dt around 7:30)</t>
-  </si>
-  <si>
-    <t>[RUSHED] BTS - BLACK SWAN (7) - DUE FRI JAN 31 9:00AM</t>
-  </si>
-  <si>
-    <t>I also have stroke MAIS YA PLZ PICK ME IM UWU (also nics dont kill ur knees 👀👀👀👀👀) BUTTT IM FREE ALL DAY feb. 8</t>
-  </si>
-  <si>
-    <t>Quynh-Nhi</t>
-  </si>
-  <si>
-    <t>Karen</t>
-  </si>
-  <si>
-    <t>After 3:30</t>
-  </si>
-  <si>
     <t>Free except 4h30-6h30</t>
   </si>
   <si>
-    <t>free after 4h30</t>
+    <t>free after 6pm</t>
+  </si>
+  <si>
+    <t>6-9pm *</t>
+  </si>
+  <si>
+    <t>6-9pm</t>
+  </si>
+  <si>
+    <t>Eli</t>
+  </si>
+  <si>
+    <t>After 7 pm</t>
+  </si>
+  <si>
+    <t>After 2:30 pm</t>
+  </si>
+  <si>
+    <t>After 2 pm</t>
+  </si>
+  <si>
+    <t>Between 4 and 8pm</t>
+  </si>
+  <si>
+    <t>aviva</t>
+  </si>
+  <si>
+    <t>free 5-9</t>
+  </si>
+  <si>
+    <t>free after 7</t>
+  </si>
+  <si>
+    <t>after5</t>
+  </si>
+  <si>
+    <t>Ruo</t>
+  </si>
+  <si>
+    <t>after 5:30pm</t>
+  </si>
+  <si>
+    <t>after 6pm</t>
+  </si>
+  <si>
+    <t>After 5 pm</t>
+  </si>
+  <si>
+    <t>Condy</t>
+  </si>
+  <si>
+    <t>After 12</t>
+  </si>
+  <si>
+    <t>Yiting</t>
+  </si>
+  <si>
+    <t>anna</t>
+  </si>
+  <si>
+    <t>IZ*ONE - FIESTA (12) - DUE SAT FEB 22 9:00PM</t>
+  </si>
+  <si>
+    <t>Between 4-8pm</t>
+  </si>
+  <si>
+    <t>In stroke, not free march 4th,8th,9th</t>
+  </si>
+  <si>
+    <t>Free feb 29 (sat) between 4 and 9pm, free march 1st after 4 pm, can manage to go to one saturday practice if necessary (but not 2)</t>
+  </si>
+  <si>
+    <t>will not be in town from feb 28 to march 8th</t>
+  </si>
+  <si>
+    <t>will leave for exchange march 30 plspls this is my goodbye fiesta</t>
+  </si>
+  <si>
+    <t>Not avail on February 24th, 28th</t>
+  </si>
+  <si>
+    <t>Unavailable on Feb 28, March 6 and 7. Starting March, I'll be free all day on Mondays and Fridays as well :)</t>
+  </si>
+  <si>
+    <t>Away from feb.28th to March 8th</t>
+  </si>
+  <si>
+    <t>in stroke, can't feb 29 (1-5pm)
+down to co-teachhh
+* would prefer not monday or tuesday night, but it's fine if it has to be</t>
+  </si>
+  <si>
+    <t>co-teach ohohoho</t>
+  </si>
+  <si>
+    <t>Before 4pm</t>
+  </si>
+  <si>
+    <t>free after 5h30pm</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This schedule applies </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ONLY</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> to the week of 23rd-29th february. Starting March, I will be free everyday until the 25th of March.</t>
+    </r>
+  </si>
+  <si>
+    <t>Hao Chen</t>
+  </si>
+  <si>
+    <t>ONLY FREE DURING MARCH BREAK AND WEEKEND BEFORE (+firday) AND AFTER (schedule ONLY applies to that), not available march 6th, I'm also teacher for Hallyu, so might have some practices TBA (but should be free after 5pm if i do have practice)</t>
+  </si>
+  <si>
+    <t>Salwa</t>
+  </si>
+  <si>
+    <t>Before 8</t>
+  </si>
+  <si>
+    <t>Cant feb 23-24-25</t>
+  </si>
+  <si>
+    <t>free 6-9pm</t>
+  </si>
+  <si>
+    <t>Free 2-8pm</t>
   </si>
 </sst>
 </file>
@@ -922,11 +1000,417 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{073F71A5-D536-2643-9891-E044647053BD}">
+  <dimension ref="A1:I14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="46.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="105.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="43" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="https://www.youtube.com/watch?v=XEhwvuOBlCA" xr:uid="{539A189F-6CF1-BB4A-AA89-BE3AB6FF2F78}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEDDD130-3FEA-B342-AB58-23B2E7542398}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D40" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -942,7 +1426,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -975,211 +1459,253 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>136</v>
+      <c r="A3" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>137</v>
+        <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>137</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="D4" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>145</v>
-      </c>
+      <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>12</v>
+        <v>140</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>11</v>
+        <v>141</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>77</v>
+        <v>142</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>77</v>
+        <v>38</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>77</v>
+        <v>143</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>11</v>
+        <v>144</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>146</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B6" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>104</v>
-      </c>
       <c r="G6" s="3" t="s">
-        <v>149</v>
+        <v>105</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>154</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="E7" s="3" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>68</v>
+        <v>151</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>68</v>
+        <v>150</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>152</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>156</v>
+        <v>12</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="D8" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="G9" s="3" t="s">
+      <c r="B10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="D11" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="https://www.youtube.com/watch?v=YVM45doZNNo" xr:uid="{5C47B52A-D8CE-DF42-8EB7-AC3FB08B613D}"/>
+    <hyperlink ref="A1" r:id="rId1" display="https://www.youtube.com/watch?v=XEhwvuOBlCA" xr:uid="{907BBE7C-5170-464D-BF4C-27BEFB2ACE2E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C96FCFC8-74A0-4B4A-A658-B299719390AA}">
   <dimension ref="A1:M8"/>
   <sheetViews>
@@ -1409,7 +1935,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6AA26D7-45B2-1A4A-91B0-76F117F9AA59}">
   <dimension ref="A1:I8"/>
   <sheetViews>
@@ -1631,7 +2157,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA89D4D5-A1AB-C148-BF69-36469C4FA223}">
   <dimension ref="A1:I11"/>
   <sheetViews>
@@ -1948,7 +2474,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926DF328-B4D7-7A40-880B-B5026507095A}">
   <dimension ref="A1:I9"/>
   <sheetViews>
@@ -2189,7 +2715,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B7F069-2B14-EB4E-B090-4721D7B9CDF9}">
   <dimension ref="A1:I7"/>
   <sheetViews>
@@ -2387,7 +2913,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74780E18-0271-3344-9AE4-771AE2C0452F}">
   <dimension ref="A1:J9"/>
   <sheetViews>

</xml_diff>

<commit_message>
seriously need to refactor lol this code is w e t
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seasy/Documents/Projects/PM-Replacement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5173D31A-5894-6342-BA33-8625954E0FB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45285F88-039B-0D47-97C3-5563EFDEFD62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{D0A65B29-C4AD-3F43-ADB3-EAE2E589548A}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="183">
   <si>
     <t>TWICE (9) - FEEL SPECIAL [SEMI-RUSH] - DUE THURS SEP 26 9:00PM</t>
   </si>
@@ -457,9 +457,6 @@
     <t>free after 6pm</t>
   </si>
   <si>
-    <t>6-9pm *</t>
-  </si>
-  <si>
     <t>6-9pm</t>
   </si>
   <si>
@@ -473,9 +470,6 @@
   </si>
   <si>
     <t>After 2 pm</t>
-  </si>
-  <si>
-    <t>Between 4 and 8pm</t>
   </si>
   <si>
     <t>aviva</t>
@@ -588,16 +582,37 @@
     <t>Salwa</t>
   </si>
   <si>
-    <t>Before 8</t>
-  </si>
-  <si>
     <t>Cant feb 23-24-25</t>
   </si>
   <si>
-    <t>free 6-9pm</t>
-  </si>
-  <si>
-    <t>Free 2-8pm</t>
+    <t>Shu</t>
+  </si>
+  <si>
+    <t>Not available before next Friday (because of school evaluations coming up). However, after that during March break I should be pretty available 😊</t>
+  </si>
+  <si>
+    <t>jess b</t>
+  </si>
+  <si>
+    <t>havent been in a cover in a while please pick meee &lt;3</t>
+  </si>
+  <si>
+    <t>free after 8h30pm</t>
+  </si>
+  <si>
+    <t>free before 1pm</t>
+  </si>
+  <si>
+    <t>free after 7pm</t>
+  </si>
+  <si>
+    <t>depends</t>
+  </si>
+  <si>
+    <t>march break(next week): unail monday 24 and friday 6pm. i only have 1 shift on next saturday so im free all day wed and thurs b4 4h45pm/fri before 6</t>
+  </si>
+  <si>
+    <t>free 2-8pm</t>
   </si>
 </sst>
 </file>
@@ -674,7 +689,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -686,6 +701,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1001,10 +1019,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{073F71A5-D536-2643-9891-E044647053BD}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:H13"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1016,12 +1034,12 @@
     <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="46.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="105.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="46.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1053,349 +1071,360 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="43" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>72</v>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>176</v>
+        <v>137</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>18</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="57" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I4" s="6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="43" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>141</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>142</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>38</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>38</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="29" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="6" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="C6" s="3" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="4" t="s">
+      <c r="I7" s="6" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="D7" s="3" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>77</v>
+      <c r="E8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="29" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="B9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="C9" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>61</v>
+      <c r="D9" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="I9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="43" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>156</v>
+      <c r="I10" s="6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="71" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>169</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>18</v>
+        <v>182</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>75</v>
+        <v>182</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>73</v>
+        <v>182</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>11</v>
+        <v>182</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>133</v>
+        <v>182</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>11</v>
+        <v>182</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>165</v>
+        <v>182</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>65</v>
+        <v>171</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>168</v>
+        <v>11</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>171</v>
+        <v>11</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="43" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>173</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>177</v>
+        <v>68</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>177</v>
+        <v>68</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>177</v>
+        <v>68</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>177</v>
+        <v>68</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>177</v>
+        <v>68</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>177</v>
+        <v>68</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>172</v>
+        <v>10</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>174</v>
+        <v>18</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>174</v>
+        <v>137</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>11</v>
+        <v>137</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>175</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1407,10 +1436,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEDDD130-3FEA-B342-AB58-23B2E7542398}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D40" sqref="A1:XFD1048576"/>
+      <selection activeCell="A17" sqref="A17:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1425,282 +1454,202 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>157</v>
-      </c>
+      <c r="A1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="4"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="3" t="s">
+      <c r="E18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>11</v>
+      <c r="G18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="43" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="https://www.youtube.com/watch?v=XEhwvuOBlCA" xr:uid="{907BBE7C-5170-464D-BF4C-27BEFB2ACE2E}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
how to tackle free 6-9
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seasy/Documents/Projects/PM-Replacement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{154E95F7-A835-794B-9857-F2D14E6D23B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EEC8E67-1CB3-BA4E-9B0A-51395D3A564F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{D0A65B29-C4AD-3F43-ADB3-EAE2E589548A}"/>
+    <workbookView xWindow="36220" yWindow="-4280" windowWidth="28800" windowHeight="17540" xr2:uid="{D0A65B29-C4AD-3F43-ADB3-EAE2E589548A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet6" sheetId="8" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="183">
   <si>
     <t>TWICE (9) - FEEL SPECIAL [SEMI-RUSH] - DUE THURS SEP 26 9:00PM</t>
   </si>
@@ -599,12 +599,27 @@
   <si>
     <t>free 2-8pm</t>
   </si>
+  <si>
+    <t>joy</t>
+  </si>
+  <si>
+    <t>after 3:30</t>
+  </si>
+  <si>
+    <t>free except 3:30-7pm</t>
+  </si>
+  <si>
+    <t>update: away from feb 28~3rd, march 5th to 7th</t>
+  </si>
+  <si>
+    <t>between 5pm-9pm</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -652,6 +667,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -674,7 +695,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -689,6 +710,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1004,10 +1026,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{073F71A5-D536-2643-9891-E044647053BD}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1340,8 +1362,8 @@
       <c r="H12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I12" s="6" t="s">
-        <v>160</v>
+      <c r="I12" s="3" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -1349,7 +1371,7 @@
         <v>143</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>144</v>
+        <v>182</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>10</v>
@@ -1361,7 +1383,7 @@
         <v>137</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>105</v>
@@ -1372,6 +1394,33 @@
       <c r="I13" s="9" t="s">
         <v>157</v>
       </c>
+    </row>
+    <row r="14" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="I14" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1386,7 +1435,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1509,7 +1558,7 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="14" spans="1:9" ht="71" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="398" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>166</v>
       </c>

</xml_diff>

<commit_message>
time to refactor code
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seasy/Documents/Projects/PM-Replacement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EEC8E67-1CB3-BA4E-9B0A-51395D3A564F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D30E52-7274-BB4E-9A71-A949AE16FCA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36220" yWindow="-4280" windowWidth="28800" windowHeight="17540" xr2:uid="{D0A65B29-C4AD-3F43-ADB3-EAE2E589548A}"/>
+    <workbookView xWindow="-100" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{D0A65B29-C4AD-3F43-ADB3-EAE2E589548A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet6" sheetId="8" r:id="rId1"/>
@@ -1028,8 +1028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{073F71A5-D536-2643-9891-E044647053BD}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add other to Schedule obj and fix create_members_from_excel()
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seasy/Documents/Projects/PM-Replacement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D30E52-7274-BB4E-9A71-A949AE16FCA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D87D8E3-41D3-6E4B-BE01-06558CF0341C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{D0A65B29-C4AD-3F43-ADB3-EAE2E589548A}"/>
+    <workbookView xWindow="-3460" yWindow="-19200" windowWidth="28800" windowHeight="17540" xr2:uid="{D0A65B29-C4AD-3F43-ADB3-EAE2E589548A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet6" sheetId="8" r:id="rId1"/>
@@ -1029,7 +1029,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>